<commit_message>
added klausen for different lifetime distr
</commit_message>
<xml_diff>
--- a/data_and_models/Make-up wells estimation and test on Hellisheidi.xlsx
+++ b/data_and_models/Make-up wells estimation and test on Hellisheidi.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrea\OneDrive - University College London\S4CE\LCA\GSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andpa\OneDrive - University College London\S4CE\GSA\Geothermal\data_and_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_9585365333247847334FEF3C11CE5229B0BBAFC5" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{C4716A13-F690-4FF9-BE1F-67B8A9581BF0}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView minimized="1" xWindow="2500" yWindow="2500" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -153,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -289,7 +290,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,6 +311,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -1966,26 +1968,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.453125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
@@ -1994,7 +1996,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -2009,7 +2011,7 @@
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2030,7 +2032,7 @@
         <v>13.154831966713166</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -2054,7 +2056,7 @@
         <v>2.1510851063829783E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -2072,12 +2074,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="E7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
         <v>3</v>
       </c>
@@ -2085,7 +2087,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="E9" t="s">
         <v>2</v>
       </c>
@@ -2093,7 +2095,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
         <v>15</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -2126,7 +2128,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -2135,17 +2137,17 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="E15" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="G16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -2163,7 +2165,7 @@
       </c>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -2187,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>26</v>
       </c>
@@ -2209,7 +2211,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E20" t="s">
         <v>3</v>
       </c>
@@ -2227,7 +2229,7 @@
         <v>21.000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E21" t="s">
         <v>15</v>
       </c>
@@ -2238,7 +2240,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
         <v>6</v>
       </c>

</xml_diff>